<commit_message>
Final changes for testing part of REF
</commit_message>
<xml_diff>
--- a/REFramework/C#/Tests/Tests.xlsx
+++ b/REFramework/C#/Tests/Tests.xlsx
@@ -1,19 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B09E86-E7F7-40F4-8A4B-0931C3A3679A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{27B09E86-E7F7-40F4-8A4B-0931C3A3679A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D576C0B1-BA92-446F-9092-387D0707F940}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
     <sheet name="Result" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Result!$A$1:$D$1</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="8">
   <si>
     <t>WorkflowFile</t>
   </si>
@@ -32,12 +29,6 @@
     <t>Success</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
     <t>Framework\CloseAllApplications.xaml</t>
   </si>
   <si>
@@ -51,13 +42,16 @@
   </si>
   <si>
     <t>SystemException</t>
+  </si>
+  <si>
+    <t>ActualResult</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,14 +62,6 @@
     <font>
       <b/>
       <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -109,10 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,7 +380,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -407,12 +394,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -420,7 +407,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -428,7 +415,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -436,15 +423,15 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -452,7 +439,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -460,7 +447,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -468,14 +455,14 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3"/>
+  <phoneticPr fontId="2"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{7198B273-8CEB-4936-858C-3C618DA468FB}">
       <formula1>"Success,BusinessException,SystemException"</formula1>
@@ -487,38 +474,94 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EEA04BB-1416-4A9D-BE28-34EECED26301}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="46.36328125" customWidth="1"/>
-    <col min="2" max="2" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.36328125" customWidth="1"/>
-    <col min="4" max="4" width="135.6328125" customWidth="1"/>
+    <col min="1" max="1" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="18.5">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="21">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <phoneticPr fontId="3"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{CB13DA15-0017-4E26-927A-C3254031AF44}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B9" xr:uid="{6CCAD5D8-F715-4488-85AA-C20AB02F763F}">
       <formula1>"Success,BusinessException,SystemException"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>